<commit_message>
media timing logic update
</commit_message>
<xml_diff>
--- a/samples/WDW Demo/WDW Demo Scenarios.xlsx
+++ b/samples/WDW Demo/WDW Demo Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DONGZ027\Desktop\Local Crafts\craft001_Soul\samples\WDW Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29E45F9-12AE-4E4B-BBD1-5D731B6FCE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EE61BE-5B3E-4F8B-846D-EC1CF43CD177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{863EB093-9973-4864-ACB4-046E3019C074}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
   <si>
     <t>Media</t>
   </si>
@@ -171,9 +171,9 @@
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -234,12 +234,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -249,20 +249,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -603,7 +606,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,7 +616,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B1" t="s">
@@ -657,7 +660,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
+      <c r="A2" s="13"/>
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -699,7 +702,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
+      <c r="A3" s="13"/>
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -741,7 +744,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
+      <c r="A4" s="13"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -783,7 +786,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -825,7 +828,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
+      <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -867,7 +870,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -909,7 +912,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
+      <c r="A8" s="13"/>
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -951,7 +954,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
+      <c r="A9" s="13"/>
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -993,7 +996,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1035,7 +1038,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
+      <c r="A11" s="13"/>
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -1077,7 +1080,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -1119,7 +1122,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
+      <c r="A13" s="13"/>
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -1161,7 +1164,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
+      <c r="A14" s="13"/>
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -1203,7 +1206,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
+      <c r="A15" s="13"/>
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -1245,7 +1248,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="13"/>
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -1299,7 +1302,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:N16"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1309,7 +1312,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
@@ -1353,7 +1356,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
+      <c r="A2" s="13"/>
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -1395,7 +1398,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
+      <c r="A3" s="13"/>
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -1437,7 +1440,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
+      <c r="A4" s="13"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -1479,7 +1482,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -1521,7 +1524,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
+      <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -1563,7 +1566,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -1605,7 +1608,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
+      <c r="A8" s="13"/>
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -1647,7 +1650,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
+      <c r="A9" s="13"/>
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -1689,7 +1692,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1731,7 +1734,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
+      <c r="A11" s="13"/>
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -1773,7 +1776,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -1815,7 +1818,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
+      <c r="A13" s="13"/>
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -1857,7 +1860,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
+      <c r="A14" s="13"/>
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -1899,7 +1902,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
+      <c r="A15" s="13"/>
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -1941,7 +1944,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="13"/>
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -2011,7 +2014,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
@@ -2055,641 +2058,641 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
+      <c r="A2" s="13"/>
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="9">
         <v>4648345.3042272096</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="9">
         <v>680665.69535436376</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="9">
         <v>4401790.3550684201</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="9">
         <v>3141834.3697368032</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="10">
         <v>1912579.268654801</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="11">
         <f>I22+$I$20/9</f>
         <v>4641526.6376336906</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="11">
         <f t="shared" ref="J2:K2" si="0">J22+$I$20/9</f>
         <v>4160794.7979576946</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="11">
         <f t="shared" si="0"/>
         <v>1957565.5959803057</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="9">
         <v>2523367.2252006899</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="9">
         <v>1651099.2023956419</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="9">
         <v>1993683.3867987189</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
+      <c r="A3" s="13"/>
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <v>967480.84594999929</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>1322422.131169999</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>38510.974419999977</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>1127007.4804599991</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>706491.49094999908</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="10">
         <v>1262482.212609998</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="9">
         <v>350080.67106999969</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="9">
         <v>1538724.6258899991</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="9">
         <v>1058300.62788</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="9">
         <v>0</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="9">
         <v>0</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
+      <c r="A4" s="13"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>109825.1819</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>156820.90499999991</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>124374.7631999999</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <v>171887.41839999991</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>169106.65289999999</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="10">
         <v>217015.74479999981</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="9">
         <v>165428.8695899999</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="9">
         <v>172894.91189999989</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="9">
         <v>224139.85189999989</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="9">
         <v>116189.9916999999</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="9">
         <v>114932.41160000001</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="9">
         <v>146112.1436999999</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>364569.53402214678</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>494746.54742613313</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="9">
         <v>286042.41476714471</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>537527.82061413443</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>560024.30891272938</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="10">
         <v>419165.40761511383</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="9">
         <v>608062.12663003558</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="9">
         <v>434388.44160499831</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="9">
         <v>551451.88271475944</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="9">
         <v>320199.48297453782</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="9">
         <v>308144.9061930991</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="9">
         <v>404043.84521597112</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
+      <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>534860.81064619415</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>993262.7863627862</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>718109.04091563553</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>1360720.7603815719</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>1363586.376303192</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <v>1148483.5071351959</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="9">
         <v>1618181.3703129671</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="9">
         <v>1707510.242428964</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="9">
         <v>1406098.4684163569</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="9">
         <v>942142.8497993073</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="9">
         <v>1198299.6036343561</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="9">
         <v>1014856.249761277</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>756739.51809999952</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>972158.76099999913</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>1150914.2802999991</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <v>1043256.457599999</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="9">
         <v>1139300.6461999989</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <v>1342031.3537999981</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="11">
         <f>I23+$I$20/9</f>
         <v>1175544.6034666656</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="11">
         <f>J23+$I$20/9</f>
         <v>1146906.9989666659</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="11">
         <f>K23+$I$20/9</f>
         <v>1599624.1253666647</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="9">
         <v>739052.90599999926</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="9">
         <v>698114.2985999994</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="9">
         <v>886390.72459999926</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
+      <c r="A8" s="13"/>
       <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>1719410.3203623211</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>2489502.950712075</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="9">
         <v>1490669.657235747</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <v>3143201.2364309821</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="9">
         <v>2973761.9281048691</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <v>3025543.75670439</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="9">
         <v>3148411.677859914</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="9">
         <v>2813910.5054344279</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="9">
         <v>3394647.0151611269</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="9">
         <v>3309396.9446717789</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="9">
         <v>1341973.9553732211</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="9">
         <v>1645342.684768283</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
+      <c r="A9" s="13"/>
       <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>750131.24023999961</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <v>964747.37894999934</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="9">
         <v>1394635.5449399981</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <v>997224.30928999837</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="9">
         <v>966119.26365999854</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="10">
         <v>1143167.3056799991</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="9">
         <v>1023893.550949999</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="9">
         <v>866992.37311999989</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="9">
         <v>1036447.944099999</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="9">
         <v>608051.38895999931</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="9">
         <v>513346.38944999961</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="9">
         <v>727992.33632999973</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
       <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>235611.09614000001</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>490763.64230999979</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="9">
         <v>718228.26823999966</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <v>505224.78973999951</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
         <v>476999.36203999969</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <v>966717.07444999984</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="9">
         <v>335457.37862999988</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="9">
         <v>597553.61669999943</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="9">
         <v>980511.1050999997</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="9">
         <v>870524.35101000022</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="9">
         <v>155326.77336999989</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="9">
         <v>243732.39186999979</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
+      <c r="A11" s="13"/>
       <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <v>1773608.587750284</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <v>2228566.0810609148</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="9">
         <v>2217031.7930739168</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="9">
         <v>2481965.8829771462</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="9">
         <v>2651696.1165219722</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <v>3027087.6623029239</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="9">
         <v>2448744.1487909579</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="9">
         <v>2454689.7190986848</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="9">
         <v>2997240.646432939</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="9">
         <v>1684559.7217549849</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="9">
         <v>1749885.9016274579</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="9">
         <v>2293560.7386077689</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
       <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="9">
         <v>109844.8004999999</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>124858.9053999999</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="9">
         <v>197825.45999999979</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="9">
         <v>196375.89199999991</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="9">
         <v>218028.37619999971</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="10">
         <v>188758.77421999979</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="9">
         <v>179040.41491999981</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="9">
         <v>200153.98819999991</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="9">
         <v>286617.4303999996</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="9">
         <v>129230.77508999981</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="9">
         <v>138079.37476999991</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="9">
         <v>128730.94439999991</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
+      <c r="A13" s="13"/>
       <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="9">
         <v>1882461.6199999989</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>2090643.0699999989</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="9">
         <v>2422842.149999998</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="9">
         <v>2460610.4799999981</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="9">
         <v>2752073.4799999972</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="10">
         <v>3098980.7338099959</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="9">
         <v>2494236.8824699949</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="9">
         <v>2564064.8362899991</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="9">
         <v>3425898.4415999982</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="9">
         <v>1652242.0779699991</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="9">
         <v>1982703.2867499981</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="9">
         <v>2771411.2068799962</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
+      <c r="A14" s="13"/>
       <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="9">
         <v>1760356.044318605</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>1946370.350636106</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="9">
         <v>2003385.5415614769</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <v>2534298.1511046519</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="9">
         <v>1889986.663212518</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="10">
         <v>2605508.8316208618</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="11">
         <f>I24+$I$20/9</f>
         <v>3101121.2686287165</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="11">
         <f>J24+$I$20/9</f>
         <v>2561096.4757382576</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="11">
         <f>K24+$I$20/9</f>
         <v>3472708.7368485094</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="9">
         <v>1821490.003038628</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="9">
         <v>1735005.976927002</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="9">
         <v>2667529.4469246641</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
+      <c r="A15" s="13"/>
       <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="9">
         <v>0</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="9">
         <v>19689.27517965595</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="9">
         <v>13102.20759243356</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="9">
         <v>0</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="9">
         <v>25553.362758078769</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <v>26518.334008503949</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="9">
         <v>22583.50344040514</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="9">
         <v>55475.694136110556</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="9">
         <v>137461.60839741741</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="9">
         <v>142960.85961392341</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="9">
         <v>1268309.1843226091</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="9">
         <v>1988087.970550854</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="13"/>
       <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="9">
         <v>405654.26832086529</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="9">
         <v>427747.06245843112</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="9">
         <v>278671.91568972089</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="9">
         <v>299071.06941083592</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="9">
         <v>330849.40697116742</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="10">
         <v>547785.99283292261</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="9">
         <v>540760.88345187122</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="9">
         <v>811856.98310840374</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="9">
         <v>692520.05223040609</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="9">
         <v>401298.9359660722</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="9">
         <v>407416.77234285278</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="9">
         <v>549495.65721643728</v>
       </c>
     </row>
@@ -2781,432 +2784,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5AFD31-E8DC-4662-826C-99A7B910C612}">
-  <dimension ref="C1:J18"/>
+  <dimension ref="D16:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
     <col min="4" max="4" width="11.7265625" customWidth="1"/>
     <col min="5" max="5" width="10.1796875" customWidth="1"/>
     <col min="6" max="6" width="10.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1">
-        <v>4474859.9709670236</v>
-      </c>
-      <c r="E1">
-        <v>3994128.1312910281</v>
-      </c>
-      <c r="F1">
-        <v>1790898.9293136389</v>
-      </c>
-      <c r="H1">
-        <f>D1*1.5</f>
-        <v>6712289.956450535</v>
-      </c>
-      <c r="I1">
-        <f t="shared" ref="I1:J1" si="0">E1*1.5</f>
-        <v>5991192.1969365422</v>
-      </c>
-      <c r="J1">
-        <f t="shared" si="0"/>
-        <v>2686348.3939704583</v>
-      </c>
-    </row>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2">
-        <v>350080.67106999969</v>
-      </c>
-      <c r="E2">
-        <v>1538724.6258899991</v>
-      </c>
-      <c r="F2">
-        <v>1058300.62788</v>
-      </c>
-      <c r="H2">
-        <f t="shared" ref="H2:H15" si="1">D2*1.5</f>
-        <v>525121.00660499954</v>
-      </c>
-      <c r="I2">
-        <f t="shared" ref="I2:I15" si="2">E2*1.5</f>
-        <v>2308086.9388349988</v>
-      </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J15" si="3">F2*1.5</f>
-        <v>1587450.9418200001</v>
-      </c>
-    </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3">
-        <v>165428.8695899999</v>
-      </c>
-      <c r="E3">
-        <v>172894.91189999989</v>
-      </c>
-      <c r="F3">
-        <v>224139.85189999989</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="1"/>
-        <v>248143.30438499985</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="2"/>
-        <v>259342.36784999984</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="3"/>
-        <v>336209.77784999984</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4">
-        <v>608062.12663003558</v>
-      </c>
-      <c r="E4">
-        <v>434388.44160499831</v>
-      </c>
-      <c r="F4">
-        <v>551451.88271475944</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>912093.18994505331</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
-        <v>651582.66240749741</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="3"/>
-        <v>827177.8240721391</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5">
-        <v>1618181.3703129671</v>
-      </c>
-      <c r="E5">
-        <v>1707510.242428964</v>
-      </c>
-      <c r="F5">
-        <v>1406098.4684163569</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>2427272.0554694505</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
-        <v>2561265.363643446</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="3"/>
-        <v>2109147.7026245352</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6">
-        <v>1008877.936799999</v>
-      </c>
-      <c r="E6">
-        <v>980240.33229999919</v>
-      </c>
-      <c r="F6">
-        <v>1432957.458699998</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>1513316.9051999985</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
-        <v>1470360.4984499989</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="3"/>
-        <v>2149436.1880499972</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7">
-        <v>3148411.677859914</v>
-      </c>
-      <c r="E7">
-        <v>2813910.5054344279</v>
-      </c>
-      <c r="F7">
-        <v>3394647.0151611269</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>4722617.5167898713</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
-        <v>4220865.758151642</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="3"/>
-        <v>5091970.5227416903</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8">
-        <v>1023893.550949999</v>
-      </c>
-      <c r="E8">
-        <v>866992.37311999989</v>
-      </c>
-      <c r="F8">
-        <v>1036447.944099999</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>1535840.3264249985</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
-        <v>1300488.5596799999</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="3"/>
-        <v>1554671.9161499985</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9">
-        <v>335457.37862999988</v>
-      </c>
-      <c r="E9">
-        <v>597553.61669999943</v>
-      </c>
-      <c r="F9">
-        <v>980511.1050999997</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>503186.06794499978</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
-        <v>896330.42504999915</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="3"/>
-        <v>1470766.6576499995</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10">
-        <v>2448744.1487909579</v>
-      </c>
-      <c r="E10">
-        <v>2454689.7190986848</v>
-      </c>
-      <c r="F10">
-        <v>2997240.646432939</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>3673116.223186437</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
-        <v>3682034.578648027</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="3"/>
-        <v>4495860.969649408</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11">
-        <v>179040.41491999981</v>
-      </c>
-      <c r="E11">
-        <v>200153.98819999991</v>
-      </c>
-      <c r="F11">
-        <v>286617.4303999996</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>268560.62237999972</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="2"/>
-        <v>300230.98229999986</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="3"/>
-        <v>429926.14559999941</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12">
-        <v>2494236.8824699949</v>
-      </c>
-      <c r="E12">
-        <v>2564064.8362899991</v>
-      </c>
-      <c r="F12">
-        <v>3425898.4415999982</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
-        <v>3741355.3237049924</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="2"/>
-        <v>3846097.2544349986</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="3"/>
-        <v>5138847.662399997</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13">
-        <v>2934454.60196205</v>
-      </c>
-      <c r="E13">
-        <v>2394429.8090715911</v>
-      </c>
-      <c r="F13">
-        <v>3306042.0701818429</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>4401681.9029430747</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="2"/>
-        <v>3591644.7136073867</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="3"/>
-        <v>4959063.1052727643</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14">
-        <v>22583.50344040514</v>
-      </c>
-      <c r="E14">
-        <v>55475.694136110556</v>
-      </c>
-      <c r="F14">
-        <v>137461.60839741741</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>33875.25516060771</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="2"/>
-        <v>83213.541204165842</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="3"/>
-        <v>206192.41259612612</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15">
-        <v>540760.88345187122</v>
-      </c>
-      <c r="E15">
-        <v>811856.98310840374</v>
-      </c>
-      <c r="F15">
-        <v>692520.05223040609</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
-        <v>811141.3251778069</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="2"/>
-        <v>1217785.4746626057</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="3"/>
-        <v>1038780.0783456091</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="D16">
-        <f>SUM(D1:F15)</f>
-        <v>65661321.730947904</v>
-      </c>
-      <c r="H16" s="1">
-        <f>SUM(H1:J15)</f>
-        <v>98491982.596421853</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D17">
-        <f>77800059-D16</f>
-        <v>12138737.269052096</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D18" s="4">
-        <f>D17/D16</f>
-        <v>0.18486891443933257</v>
-      </c>
+    <row r="16" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D18" s="4"/>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
media timing updated to 52+ weeks
</commit_message>
<xml_diff>
--- a/samples/WDW Demo/WDW Demo Scenarios.xlsx
+++ b/samples/WDW Demo/WDW Demo Scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DONGZ027\Desktop\Local Crafts\craft001_Soul\samples\WDW Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EE61BE-5B3E-4F8B-846D-EC1CF43CD177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217C6FC5-D149-4730-AA54-E4E41EBAA16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{863EB093-9973-4864-ACB4-046E3019C074}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{863EB093-9973-4864-ACB4-046E3019C074}"/>
   </bookViews>
   <sheets>
     <sheet name="FY24" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
   <si>
     <t>Media</t>
   </si>
@@ -153,9 +153,6 @@
 Start with evenly distribute among {TV, Streaming, Social}
 Target 1: 1,915,962 (+1.2%)
 Target 2: 1,931,107 (+2%)</t>
-  </si>
-  <si>
-    <t>3072508.3948838C2:L13A1C2:J12C2:N12C2:O12C2:N13C2:M14C2:M15C2:M16C2:N16C2:N17C2:N16</t>
   </si>
   <si>
     <t>Scenrio 0:  
@@ -257,14 +254,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -605,19 +602,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E73F9B6-A2E4-4D87-9375-0EBE2B5AB6DC}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>37</v>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -659,8 +656,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -701,8 +698,8 @@
         <v>1993683.3867987189</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -743,8 +740,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -785,8 +782,8 @@
         <v>146112.1436999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -827,8 +824,8 @@
         <v>404043.84521597112</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -869,8 +866,8 @@
         <v>1014856.249761277</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -911,8 +908,8 @@
         <v>886390.72459999926</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -953,8 +950,8 @@
         <v>1645342.684768283</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -995,8 +992,8 @@
         <v>727992.33632999973</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1037,8 +1034,8 @@
         <v>243732.39186999979</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -1079,8 +1076,8 @@
         <v>2293560.7386077689</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -1121,8 +1118,8 @@
         <v>128730.94439999991</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -1163,8 +1160,8 @@
         <v>2771411.2068799962</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -1205,8 +1202,8 @@
         <v>2667529.4469246641</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -1247,8 +1244,8 @@
         <v>1988087.970550854</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -1305,14 +1302,14 @@
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
@@ -1355,8 +1352,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -1397,8 +1394,8 @@
         <v>2193051.7257000003</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -1439,8 +1436,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -1481,8 +1478,8 @@
         <v>160723.35806999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -1523,8 +1520,8 @@
         <v>444448.22972</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -1565,8 +1562,8 @@
         <v>1116341.875</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -1607,8 +1604,8 @@
         <v>975029.79706000001</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -1649,8 +1646,8 @@
         <v>1809876.9535000003</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -1691,8 +1688,8 @@
         <v>800791.56993</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1733,8 +1730,8 @@
         <v>268105.63108999998</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -1775,8 +1772,8 @@
         <v>2522916.8129000003</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -1817,8 +1814,8 @@
         <v>141604.03883999999</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -1859,8 +1856,8 @@
         <v>3048552.3277000003</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -1901,8 +1898,8 @@
         <v>2934282.3917000005</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -1943,8 +1940,8 @@
         <v>2186896.7681</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -1997,24 +1994,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523EDD69-6A09-489B-874D-780A72043A43}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="C2:N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.81640625" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.08984375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" customWidth="1"/>
-    <col min="12" max="14" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
@@ -2057,13 +2055,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>36</v>
+      <c r="C2" s="9">
+        <v>3072508.3948837989</v>
       </c>
       <c r="D2" s="9">
         <v>4648345.3042272096</v>
@@ -2102,8 +2100,8 @@
         <v>1993683.3867987189</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -2144,8 +2142,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -2186,8 +2184,8 @@
         <v>146112.1436999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -2228,8 +2226,8 @@
         <v>404043.84521597112</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -2270,8 +2268,8 @@
         <v>1014856.249761277</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -2315,8 +2313,8 @@
         <v>886390.72459999926</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -2357,8 +2355,8 @@
         <v>1645342.684768283</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -2399,8 +2397,8 @@
         <v>727992.33632999973</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -2441,8 +2439,8 @@
         <v>243732.39186999979</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -2483,8 +2481,8 @@
         <v>2293560.7386077689</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -2525,8 +2523,8 @@
         <v>128730.94439999991</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -2567,8 +2565,8 @@
         <v>2771411.2068799962</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -2612,8 +2610,8 @@
         <v>2667529.4469246641</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -2654,8 +2652,8 @@
         <v>1988087.970550854</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -2696,7 +2694,7 @@
         <v>549495.65721643728</v>
       </c>
     </row>
-    <row r="18" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H18" s="8" t="s">
         <v>16</v>
       </c>
@@ -2708,7 +2706,7 @@
         <v>166666.66666666666</v>
       </c>
     </row>
-    <row r="19" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H19" s="8" t="s">
         <v>18</v>
       </c>
@@ -2720,7 +2718,7 @@
         <v>1931107.2933234449</v>
       </c>
     </row>
-    <row r="20" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H20" s="7" t="s">
         <v>17</v>
       </c>
@@ -2732,7 +2730,7 @@
         <v>2.2844499020996872E-2</v>
       </c>
     </row>
-    <row r="22" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H22" s="6" t="s">
         <v>14</v>
       </c>
@@ -2746,7 +2744,7 @@
         <v>1790898.9293136389</v>
       </c>
     </row>
-    <row r="23" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H23" s="6" t="s">
         <v>13</v>
       </c>
@@ -2760,7 +2758,7 @@
         <v>1432957.458699998</v>
       </c>
     </row>
-    <row r="24" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H24" s="6" t="s">
         <v>15</v>
       </c>
@@ -2790,26 +2788,26 @@
       <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H16" s="1"/>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>